<commit_message>
Update - Changes based on the last meeting
</commit_message>
<xml_diff>
--- a/DataIn/VarExpl/Puntos_moranza.xlsx
+++ b/DataIn/VarExpl/Puntos_moranza.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a6b088a06617d4fb/Ejercicio 7/Documents/Documents/Maestria/Modelado_Merlin/GitHub_Datos/Social_Model_Enchugal/DataIn/VarExpl/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{129E234C-EA85-4BF4-B6FC-6210C0AED57A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B76402B5-578E-4148-9B8A-3E67C3061D34}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="8_{129E234C-EA85-4BF4-B6FC-6210C0AED57A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{18A173F7-3290-41D5-BC32-E897914899E1}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{28AC0027-66F0-44D4-B2F1-AD053B04A632}"/>
+    <workbookView xWindow="-28920" yWindow="-990" windowWidth="29040" windowHeight="15720" xr2:uid="{28AC0027-66F0-44D4-B2F1-AD053B04A632}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$131</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -500,6 +503,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -821,8 +828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{663AE616-5976-4A00-8446-0A108E968D61}">
   <dimension ref="A1:D131"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="F60" sqref="F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -847,67 +854,67 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>74</v>
+        <v>107</v>
       </c>
       <c r="B2">
-        <v>-15.433439999999999</v>
+        <v>-15.435484000000001</v>
       </c>
       <c r="C2" s="1">
-        <v>12.049491</v>
+        <v>12.045779</v>
       </c>
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>75</v>
+        <v>48</v>
       </c>
       <c r="B3">
-        <v>-15.433439999999999</v>
+        <v>-15.443038</v>
       </c>
       <c r="C3" s="1">
-        <v>12.049491</v>
+        <v>12.032499</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>76</v>
+        <v>41</v>
       </c>
       <c r="B4">
-        <v>-15.433439999999999</v>
+        <v>-15.433437</v>
       </c>
       <c r="C4" s="1">
-        <v>12.049491</v>
+        <v>12.043043000000001</v>
       </c>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>77</v>
+        <v>44</v>
       </c>
       <c r="B5">
-        <v>-15.433439999999999</v>
+        <v>-15.432326</v>
       </c>
       <c r="C5" s="1">
-        <v>12.049491</v>
+        <v>12.043132</v>
       </c>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>78</v>
+        <v>123</v>
       </c>
       <c r="B6">
-        <v>-15.433439999999999</v>
+        <v>-15.442837000000001</v>
       </c>
       <c r="C6" s="1">
-        <v>12.049491</v>
+        <v>12.025421</v>
       </c>
       <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B7">
         <v>-15.433439999999999</v>
@@ -919,55 +926,55 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="B8">
-        <v>-15.432475</v>
+        <v>-15.444051999999999</v>
       </c>
       <c r="C8" s="1">
-        <v>12.049398999999999</v>
+        <v>12.036472</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>1</v>
+        <v>104</v>
       </c>
       <c r="B9">
-        <v>-15.437564999999999</v>
+        <v>-15.441848999999999</v>
       </c>
       <c r="C9" s="1">
-        <v>12.047115</v>
+        <v>12.048705</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>80</v>
+        <v>35</v>
       </c>
       <c r="B10">
-        <v>-15.437564999999999</v>
+        <v>-15.440213999999999</v>
       </c>
       <c r="C10" s="1">
-        <v>12.047115</v>
+        <v>12.050008</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>2</v>
+        <v>131</v>
       </c>
       <c r="B11">
-        <v>-15.437564999999999</v>
+        <v>-15.44149</v>
       </c>
       <c r="C11" s="1">
-        <v>12.047115</v>
+        <v>12.025423999999999</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B12">
         <v>-15.437564999999999</v>
@@ -979,127 +986,127 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="B13">
-        <v>-15.437564999999999</v>
+        <v>-15.44149</v>
       </c>
       <c r="C13" s="1">
-        <v>12.047115</v>
+        <v>12.025423999999999</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>4</v>
+        <v>127</v>
       </c>
       <c r="B14">
-        <v>-15.437564999999999</v>
+        <v>-15.447722000000001</v>
       </c>
       <c r="C14" s="1">
-        <v>12.047115</v>
+        <v>12.028575999999999</v>
       </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>5</v>
+        <v>124</v>
       </c>
       <c r="B15">
-        <v>-15.437564999999999</v>
+        <v>-15.442837000000001</v>
       </c>
       <c r="C15" s="1">
-        <v>12.047115</v>
+        <v>12.025421</v>
       </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>6</v>
+        <v>54</v>
       </c>
       <c r="B16">
-        <v>-15.437564999999999</v>
+        <v>-15.444051999999999</v>
       </c>
       <c r="C16" s="1">
-        <v>12.047115</v>
+        <v>12.036472</v>
       </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="B17">
-        <v>-15.437564999999999</v>
+        <v>-15.431507999999999</v>
       </c>
       <c r="C17" s="1">
-        <v>12.047115</v>
+        <v>12.03773</v>
       </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>7</v>
+        <v>88</v>
       </c>
       <c r="B18">
-        <v>-15.437564999999999</v>
+        <v>-15.435999000000001</v>
       </c>
       <c r="C18" s="1">
-        <v>12.047115</v>
+        <v>12.049841000000001</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>8</v>
+        <v>98</v>
       </c>
       <c r="B19">
-        <v>-15.442026</v>
+        <v>-15.435093</v>
       </c>
       <c r="C19" s="1">
-        <v>12.048022</v>
+        <v>12.046393</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>83</v>
+        <v>129</v>
       </c>
       <c r="B20">
-        <v>-15.442026</v>
+        <v>-15.442506</v>
       </c>
       <c r="C20" s="1">
-        <v>12.048022</v>
+        <v>12.026863000000001</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>9</v>
+        <v>62</v>
       </c>
       <c r="B21">
-        <v>-15.442026</v>
+        <v>-15.44309</v>
       </c>
       <c r="C21" s="1">
-        <v>12.048022</v>
+        <v>12.026223</v>
       </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>84</v>
+        <v>130</v>
       </c>
       <c r="B22">
-        <v>-15.442026</v>
+        <v>-15.442506</v>
       </c>
       <c r="C22" s="1">
-        <v>12.048022</v>
+        <v>12.026863000000001</v>
       </c>
       <c r="D22" s="1"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>85</v>
+        <v>8</v>
       </c>
       <c r="B23">
         <v>-15.442026</v>
@@ -1111,499 +1118,499 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B24">
-        <v>-15.442026</v>
+        <v>-15.437514999999999</v>
       </c>
       <c r="C24" s="1">
-        <v>12.048022</v>
+        <v>12.044644999999999</v>
       </c>
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>11</v>
+        <v>105</v>
       </c>
       <c r="B25">
-        <v>-15.439249999999999</v>
+        <v>-15.441848999999999</v>
       </c>
       <c r="C25" s="1">
-        <v>12.048765</v>
+        <v>12.048705</v>
       </c>
       <c r="D25" s="1"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>86</v>
+        <v>115</v>
       </c>
       <c r="B26">
-        <v>-15.439249999999999</v>
+        <v>-15.445966</v>
       </c>
       <c r="C26" s="1">
-        <v>12.048765</v>
+        <v>12.036759</v>
       </c>
       <c r="D26" s="1"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B27">
-        <v>-15.439249999999999</v>
+        <v>-15.437817000000001</v>
       </c>
       <c r="C27" s="1">
-        <v>12.048765</v>
+        <v>12.045349</v>
       </c>
       <c r="D27" s="1"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>13</v>
+        <v>99</v>
       </c>
       <c r="B28">
-        <v>-15.441048</v>
+        <v>-15.435093</v>
       </c>
       <c r="C28" s="1">
-        <v>12.048957</v>
+        <v>12.046393</v>
       </c>
       <c r="D28" s="1"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="B29">
-        <v>-15.441048</v>
+        <v>-15.437093000000001</v>
       </c>
       <c r="C29" s="1">
-        <v>12.048957</v>
+        <v>12.046369</v>
       </c>
       <c r="D29" s="1"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>14</v>
+        <v>83</v>
       </c>
       <c r="B30">
-        <v>-15.437502</v>
+        <v>-15.442026</v>
       </c>
       <c r="C30" s="1">
-        <v>12.049643</v>
+        <v>12.048022</v>
       </c>
       <c r="D30" s="1"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="B31">
-        <v>-15.437514999999999</v>
+        <v>-15.439328</v>
       </c>
       <c r="C31" s="1">
-        <v>12.044644999999999</v>
+        <v>12.027585</v>
       </c>
       <c r="D31" s="1"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="B32">
-        <v>-15.431424</v>
+        <v>-15.433439999999999</v>
       </c>
       <c r="C32" s="1">
-        <v>12.049054</v>
+        <v>12.049491</v>
       </c>
       <c r="D32" s="1"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>17</v>
+        <v>80</v>
       </c>
       <c r="B33">
-        <v>-15.431424</v>
+        <v>-15.437564999999999</v>
       </c>
       <c r="C33" s="1">
-        <v>12.049054</v>
+        <v>12.047115</v>
       </c>
       <c r="D33" s="1"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>88</v>
+        <v>37</v>
       </c>
       <c r="B34">
-        <v>-15.435999000000001</v>
+        <v>-15.435484000000001</v>
       </c>
       <c r="C34" s="1">
-        <v>12.049841000000001</v>
+        <v>12.045779</v>
       </c>
       <c r="D34" s="1"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>89</v>
+        <v>2</v>
       </c>
       <c r="B35">
-        <v>-15.435999000000001</v>
+        <v>-15.437564999999999</v>
       </c>
       <c r="C35" s="1">
-        <v>12.049841000000001</v>
+        <v>12.047115</v>
       </c>
       <c r="D35" s="1"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>18</v>
+        <v>117</v>
       </c>
       <c r="B36">
-        <v>-15.435999000000001</v>
+        <v>-15.441803</v>
       </c>
       <c r="C36" s="1">
-        <v>12.049841000000001</v>
+        <v>12.035795999999999</v>
       </c>
       <c r="D36" s="1"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="B37">
-        <v>-15.435999000000001</v>
+        <v>-15.437564999999999</v>
       </c>
       <c r="C37" s="1">
-        <v>12.049841000000001</v>
+        <v>12.047115</v>
       </c>
       <c r="D37" s="1"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>90</v>
+        <v>49</v>
       </c>
       <c r="B38">
-        <v>-15.435999000000001</v>
+        <v>-15.445504</v>
       </c>
       <c r="C38" s="1">
-        <v>12.049841000000001</v>
+        <v>12.031674000000001</v>
       </c>
       <c r="D38" s="1"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>20</v>
+        <v>101</v>
       </c>
       <c r="B39">
-        <v>-15.435999000000001</v>
+        <v>-15.437093000000001</v>
       </c>
       <c r="C39" s="1">
-        <v>12.049841000000001</v>
+        <v>12.046369</v>
       </c>
       <c r="D39" s="1"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>21</v>
+        <v>81</v>
       </c>
       <c r="B40">
-        <v>-15.435999000000001</v>
+        <v>-15.437564999999999</v>
       </c>
       <c r="C40" s="1">
-        <v>12.049841000000001</v>
+        <v>12.047115</v>
       </c>
       <c r="D40" s="1"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>22</v>
+        <v>128</v>
       </c>
       <c r="B41">
-        <v>-15.435999000000001</v>
+        <v>-15.447526</v>
       </c>
       <c r="C41" s="1">
-        <v>12.049841000000001</v>
+        <v>12.028841999999999</v>
       </c>
       <c r="D41" s="1"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="B42">
-        <v>-15.435999000000001</v>
+        <v>-15.439249999999999</v>
       </c>
       <c r="C42" s="1">
-        <v>12.049841000000001</v>
+        <v>12.048765</v>
       </c>
       <c r="D42" s="1"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>91</v>
+        <v>60</v>
       </c>
       <c r="B43">
-        <v>-15.434558000000001</v>
+        <v>-15.439328</v>
       </c>
       <c r="C43" s="1">
-        <v>12.046099999999999</v>
+        <v>12.027585</v>
       </c>
       <c r="D43" s="1"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="B44">
-        <v>-15.437817000000001</v>
+        <v>-15.432672</v>
       </c>
       <c r="C44" s="1">
-        <v>12.045349</v>
+        <v>12.041442</v>
       </c>
       <c r="D44" s="1"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>92</v>
+        <v>50</v>
       </c>
       <c r="B45">
-        <v>-15.437817000000001</v>
+        <v>-15.445504</v>
       </c>
       <c r="C45" s="1">
-        <v>12.045349</v>
+        <v>12.031674000000001</v>
       </c>
       <c r="D45" s="1"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="B46">
-        <v>-15.43183</v>
+        <v>-15.435442</v>
       </c>
       <c r="C46" s="1">
-        <v>12.04955</v>
+        <v>12.050136999999999</v>
       </c>
       <c r="D46" s="1"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="B47">
-        <v>-15.43183</v>
+        <v>-15.442026</v>
       </c>
       <c r="C47" s="1">
-        <v>12.04955</v>
+        <v>12.048022</v>
       </c>
       <c r="D47" s="1"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="B48">
-        <v>-15.43183</v>
+        <v>-15.442026</v>
       </c>
       <c r="C48" s="1">
-        <v>12.04955</v>
+        <v>12.048022</v>
       </c>
       <c r="D48" s="1"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>95</v>
+        <v>31</v>
       </c>
       <c r="B49">
-        <v>-15.43183</v>
+        <v>-15.436031</v>
       </c>
       <c r="C49" s="1">
-        <v>12.04955</v>
+        <v>12.046004</v>
       </c>
       <c r="D49" s="1"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>26</v>
+        <v>89</v>
       </c>
       <c r="B50">
-        <v>-15.440300000000001</v>
+        <v>-15.435999000000001</v>
       </c>
       <c r="C50" s="1">
-        <v>12.049073</v>
+        <v>12.049841000000001</v>
       </c>
       <c r="D50" s="1"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>96</v>
+        <v>65</v>
       </c>
       <c r="B51">
-        <v>-15.440303999999999</v>
+        <v>-15.447526</v>
       </c>
       <c r="C51" s="1">
-        <v>12.050242000000001</v>
+        <v>12.028841999999999</v>
       </c>
       <c r="D51" s="1"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>97</v>
+        <v>38</v>
       </c>
       <c r="B52">
-        <v>-15.44023</v>
+        <v>-15.435484000000001</v>
       </c>
       <c r="C52" s="1">
-        <v>12.04865</v>
+        <v>12.045779</v>
       </c>
       <c r="D52" s="1"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>98</v>
+        <v>13</v>
       </c>
       <c r="B53">
-        <v>-15.435093</v>
+        <v>-15.441048</v>
       </c>
       <c r="C53" s="1">
-        <v>12.046393</v>
+        <v>12.048957</v>
       </c>
       <c r="D53" s="1"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>99</v>
+        <v>45</v>
       </c>
       <c r="B54">
-        <v>-15.435093</v>
+        <v>-15.432615</v>
       </c>
       <c r="C54" s="1">
-        <v>12.046393</v>
+        <v>12.040514999999999</v>
       </c>
       <c r="D54" s="1"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>27</v>
+        <v>93</v>
       </c>
       <c r="B55">
-        <v>-15.435093</v>
+        <v>-15.43183</v>
       </c>
       <c r="C55" s="1">
-        <v>12.046393</v>
+        <v>12.04955</v>
       </c>
       <c r="D55" s="1"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="B56">
-        <v>-15.435093</v>
+        <v>-15.437564999999999</v>
       </c>
       <c r="C56" s="1">
-        <v>12.046393</v>
+        <v>12.047115</v>
       </c>
       <c r="D56" s="1"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>100</v>
+        <v>126</v>
       </c>
       <c r="B57">
-        <v>-15.437093000000001</v>
+        <v>-15.446236000000001</v>
       </c>
       <c r="C57" s="1">
-        <v>12.046369</v>
+        <v>12.037397</v>
       </c>
       <c r="D57" s="1"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>101</v>
+        <v>16</v>
       </c>
       <c r="B58">
-        <v>-15.437093000000001</v>
+        <v>-15.431424</v>
       </c>
       <c r="C58" s="1">
-        <v>12.046369</v>
+        <v>12.049054</v>
       </c>
       <c r="D58" s="1"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>29</v>
+        <v>86</v>
       </c>
       <c r="B59">
-        <v>-15.437093000000001</v>
+        <v>-15.439249999999999</v>
       </c>
       <c r="C59" s="1">
-        <v>12.046369</v>
+        <v>12.048765</v>
       </c>
       <c r="D59" s="1"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>102</v>
+        <v>18</v>
       </c>
       <c r="B60">
-        <v>-15.437093000000001</v>
+        <v>-15.435999000000001</v>
       </c>
       <c r="C60" s="1">
-        <v>12.046369</v>
+        <v>12.049841000000001</v>
       </c>
       <c r="D60" s="1"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>103</v>
+        <v>58</v>
       </c>
       <c r="B61">
-        <v>-15.437093000000001</v>
+        <v>-15.443918999999999</v>
       </c>
       <c r="C61" s="1">
-        <v>12.046369</v>
+        <v>12.037611999999999</v>
       </c>
       <c r="D61" s="1"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>30</v>
+        <v>125</v>
       </c>
       <c r="B62">
-        <v>-15.437093000000001</v>
+        <v>-15.441784999999999</v>
       </c>
       <c r="C62" s="1">
-        <v>12.046369</v>
+        <v>12.034478</v>
       </c>
       <c r="D62" s="1"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B63">
-        <v>-15.436031</v>
+        <v>-15.435093</v>
       </c>
       <c r="C63" s="1">
-        <v>12.046004</v>
+        <v>12.046393</v>
       </c>
       <c r="D63" s="1"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>32</v>
+        <v>85</v>
       </c>
       <c r="B64">
-        <v>-15.436031</v>
+        <v>-15.442026</v>
       </c>
       <c r="C64" s="1">
-        <v>12.046004</v>
+        <v>12.048022</v>
       </c>
       <c r="D64" s="1"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B65">
         <v>-15.436031</v>
@@ -1615,403 +1622,403 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>34</v>
+        <v>119</v>
       </c>
       <c r="B66">
-        <v>-15.436031</v>
+        <v>-15.445504</v>
       </c>
       <c r="C66" s="1">
-        <v>12.046004</v>
+        <v>12.031674000000001</v>
       </c>
       <c r="D66" s="1"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>104</v>
+        <v>25</v>
       </c>
       <c r="B67">
-        <v>-15.441848999999999</v>
+        <v>-15.43183</v>
       </c>
       <c r="C67" s="1">
-        <v>12.048705</v>
+        <v>12.04955</v>
       </c>
       <c r="D67" s="1"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>105</v>
+        <v>51</v>
       </c>
       <c r="B68">
-        <v>-15.441848999999999</v>
+        <v>-15.445504</v>
       </c>
       <c r="C68" s="1">
-        <v>12.048705</v>
+        <v>12.031674000000001</v>
       </c>
       <c r="D68" s="1"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>106</v>
+        <v>56</v>
       </c>
       <c r="B69">
-        <v>-15.435442</v>
+        <v>-15.441229</v>
       </c>
       <c r="C69" s="1">
-        <v>12.050136999999999</v>
+        <v>12.026527</v>
       </c>
       <c r="D69" s="1"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="B70">
-        <v>-15.440213999999999</v>
+        <v>-15.435999000000001</v>
       </c>
       <c r="C70" s="1">
-        <v>12.050008</v>
+        <v>12.049841000000001</v>
       </c>
       <c r="D70" s="1"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>36</v>
+        <v>116</v>
       </c>
       <c r="B71">
-        <v>-15.436559000000001</v>
+        <v>-15.450462999999999</v>
       </c>
       <c r="C71" s="1">
-        <v>12.044413</v>
+        <v>12.031342</v>
       </c>
       <c r="D71" s="1"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="B72">
-        <v>-15.45335</v>
+        <v>-15.44023</v>
       </c>
       <c r="C72" s="1">
-        <v>12.045925</v>
+        <v>12.04865</v>
       </c>
       <c r="D72" s="1"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="B73">
-        <v>-15.45335</v>
+        <v>-15.431424</v>
       </c>
       <c r="C73" s="1">
-        <v>12.045925</v>
+        <v>12.049054</v>
       </c>
       <c r="D73" s="1"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>38</v>
+        <v>121</v>
       </c>
       <c r="B74">
-        <v>-15.45335</v>
+        <v>-15.439328</v>
       </c>
       <c r="C74" s="1">
-        <v>12.045925</v>
+        <v>12.027585</v>
       </c>
       <c r="D74" s="1"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B75">
-        <v>-15.45335</v>
+        <v>-15.433437</v>
       </c>
       <c r="C75" s="1">
-        <v>12.045925</v>
+        <v>12.043043000000001</v>
       </c>
       <c r="D75" s="1"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="B76">
-        <v>-15.431891</v>
+        <v>-15.430158</v>
       </c>
       <c r="C76" s="1">
-        <v>12.042702999999999</v>
+        <v>12.046714</v>
       </c>
       <c r="D76" s="1"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
-        <v>109</v>
+        <v>63</v>
       </c>
       <c r="B77">
-        <v>-15.431891</v>
+        <v>-15.441784999999999</v>
       </c>
       <c r="C77" s="1">
-        <v>12.042702999999999</v>
+        <v>12.034478</v>
       </c>
       <c r="D77" s="1"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B78">
-        <v>-15.432672</v>
+        <v>-15.433437</v>
       </c>
       <c r="C78" s="1">
-        <v>12.041442</v>
+        <v>12.043043000000001</v>
       </c>
       <c r="D78" s="1"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="B79">
-        <v>-15.432672</v>
+        <v>-15.43183</v>
       </c>
       <c r="C79" s="1">
-        <v>12.041442</v>
+        <v>12.04955</v>
       </c>
       <c r="D79" s="1"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B80">
-        <v>-15.432672</v>
+        <v>-15.431891</v>
       </c>
       <c r="C80" s="1">
-        <v>12.041442</v>
+        <v>12.042702999999999</v>
       </c>
       <c r="D80" s="1"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B81">
-        <v>15.433437</v>
+        <v>-15.436031</v>
       </c>
       <c r="C81" s="1">
-        <v>12.043043000000001</v>
+        <v>12.046004</v>
       </c>
       <c r="D81" s="1"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="B82">
-        <v>15.433437</v>
+        <v>-15.44149</v>
       </c>
       <c r="C82" s="1">
-        <v>12.043043000000001</v>
+        <v>12.025423999999999</v>
       </c>
       <c r="D82" s="1"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="B83">
-        <v>15.433437</v>
+        <v>-15.445065</v>
       </c>
       <c r="C83" s="1">
-        <v>12.043043000000001</v>
+        <v>12.029987999999999</v>
       </c>
       <c r="D83" s="1"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="B84">
-        <v>-15.432326</v>
+        <v>-15.447526</v>
       </c>
       <c r="C84" s="1">
-        <v>12.043132</v>
+        <v>12.028841999999999</v>
       </c>
       <c r="D84" s="1"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="B85">
-        <v>15.432615</v>
+        <v>-15.435999000000001</v>
       </c>
       <c r="C85" s="1">
-        <v>12.040514999999999</v>
+        <v>12.049841000000001</v>
       </c>
       <c r="D85" s="1"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
-        <v>112</v>
+        <v>76</v>
       </c>
       <c r="B86">
-        <v>15.432615</v>
+        <v>-15.433439999999999</v>
       </c>
       <c r="C86" s="1">
-        <v>12.040514999999999</v>
+        <v>12.049491</v>
       </c>
       <c r="D86" s="1"/>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
-        <v>46</v>
+        <v>109</v>
       </c>
       <c r="B87">
-        <v>-15.431507999999999</v>
+        <v>-15.431891</v>
       </c>
       <c r="C87" s="1">
-        <v>12.03773</v>
+        <v>12.042702999999999</v>
       </c>
       <c r="D87" s="1"/>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="B88">
-        <v>-15.430459000000001</v>
+        <v>-15.435999000000001</v>
       </c>
       <c r="C88" s="1">
-        <v>12.037611999999999</v>
+        <v>12.049841000000001</v>
       </c>
       <c r="D88" s="1"/>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="B89">
-        <v>-15.430158</v>
+        <v>-15.43183</v>
       </c>
       <c r="C89" s="1">
-        <v>12.046714</v>
+        <v>12.04955</v>
       </c>
       <c r="D89" s="1"/>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="B90">
-        <v>-15.430158</v>
+        <v>-15.446011</v>
       </c>
       <c r="C90" s="1">
-        <v>12.046714</v>
+        <v>12.029113799999999</v>
       </c>
       <c r="D90" s="1"/>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
-        <v>115</v>
+        <v>21</v>
       </c>
       <c r="B91">
-        <v>-15.445966</v>
+        <v>-15.435999000000001</v>
       </c>
       <c r="C91" s="1">
-        <v>12.036759</v>
+        <v>12.049841000000001</v>
       </c>
       <c r="D91" s="1"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="B92">
-        <v>-15.443038</v>
+        <v>-15.44149</v>
       </c>
       <c r="C92" s="1">
-        <v>12.032499</v>
+        <v>12.025423999999999</v>
       </c>
       <c r="D92" s="1"/>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="B93">
-        <v>-15.450462999999999</v>
+        <v>-15.440303999999999</v>
       </c>
       <c r="C93" s="1">
-        <v>12.031342</v>
+        <v>12.050242000000001</v>
       </c>
       <c r="D93" s="1"/>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B94">
-        <v>-15.441803</v>
+        <v>-15.445504</v>
       </c>
       <c r="C94" s="1">
-        <v>12.035795999999999</v>
+        <v>12.031674000000001</v>
       </c>
       <c r="D94" s="1"/>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
-        <v>118</v>
+        <v>22</v>
       </c>
       <c r="B95">
-        <v>-15.444051999999999</v>
+        <v>-15.435999000000001</v>
       </c>
       <c r="C95" s="1">
-        <v>12.036472</v>
+        <v>12.049841000000001</v>
       </c>
       <c r="D95" s="1"/>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
-        <v>49</v>
+        <v>0</v>
       </c>
       <c r="B96">
-        <v>-15.445504</v>
+        <v>-15.432475</v>
       </c>
       <c r="C96" s="1">
-        <v>12.031674000000001</v>
+        <v>12.049398999999999</v>
       </c>
       <c r="D96" s="1"/>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="B97">
-        <v>-15.445504</v>
+        <v>-15.437502</v>
       </c>
       <c r="C97" s="1">
-        <v>12.031674000000001</v>
+        <v>12.049643</v>
       </c>
       <c r="D97" s="1"/>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
-        <v>119</v>
+        <v>5</v>
       </c>
       <c r="B98">
-        <v>-15.445504</v>
+        <v>-15.437564999999999</v>
       </c>
       <c r="C98" s="1">
-        <v>12.031674000000001</v>
+        <v>12.047115</v>
       </c>
       <c r="D98" s="1"/>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B99">
         <v>-15.445504</v>
@@ -2023,43 +2030,43 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
-        <v>120</v>
+        <v>6</v>
       </c>
       <c r="B100">
-        <v>-15.445504</v>
+        <v>-15.437564999999999</v>
       </c>
       <c r="C100" s="1">
-        <v>12.031674000000001</v>
+        <v>12.047115</v>
       </c>
       <c r="D100" s="1"/>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
-        <v>52</v>
+        <v>112</v>
       </c>
       <c r="B101">
-        <v>-15.445504</v>
+        <v>-15.432615</v>
       </c>
       <c r="C101" s="1">
-        <v>12.031674000000001</v>
+        <v>12.040514999999999</v>
       </c>
       <c r="D101" s="1"/>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="B102">
-        <v>-15.444051999999999</v>
+        <v>-15.437093000000001</v>
       </c>
       <c r="C102" s="1">
-        <v>12.036472</v>
+        <v>12.046369</v>
       </c>
       <c r="D102" s="1"/>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B103">
         <v>-15.444051999999999</v>
@@ -2071,341 +2078,346 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
-        <v>55</v>
+        <v>102</v>
       </c>
       <c r="B104">
-        <v>-15.444051999999999</v>
+        <v>-15.437093000000001</v>
       </c>
       <c r="C104" s="1">
-        <v>12.036472</v>
+        <v>12.046369</v>
       </c>
       <c r="D104" s="1"/>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="B105">
-        <v>-15.441229</v>
+        <v>-15.430459000000001</v>
       </c>
       <c r="C105" s="1">
-        <v>12.026527</v>
+        <v>12.037611999999999</v>
       </c>
       <c r="D105" s="1"/>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="B106">
-        <v>-15.441229</v>
+        <v>-15.439432</v>
       </c>
       <c r="C106" s="1">
-        <v>12.026527</v>
+        <v>12.025613</v>
       </c>
       <c r="D106" s="1"/>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="B107">
-        <v>-15.443918999999999</v>
+        <v>-15.442218</v>
       </c>
       <c r="C107" s="1">
-        <v>12.037611999999999</v>
+        <v>12.035133</v>
       </c>
       <c r="D107" s="1"/>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
-        <v>59</v>
+        <v>114</v>
       </c>
       <c r="B108">
-        <v>-15.439328</v>
+        <v>-15.430158</v>
       </c>
       <c r="C108" s="1">
-        <v>12.027585</v>
+        <v>12.046714</v>
       </c>
       <c r="D108" s="1"/>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="B109">
-        <v>-15.439328</v>
+        <v>-15.433439999999999</v>
       </c>
       <c r="C109" s="1">
-        <v>12.027585</v>
+        <v>12.049491</v>
       </c>
       <c r="D109" s="1"/>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
-        <v>121</v>
+        <v>39</v>
       </c>
       <c r="B110">
-        <v>-15.439328</v>
+        <v>-15.435484000000001</v>
       </c>
       <c r="C110" s="1">
-        <v>12.027585</v>
+        <v>12.045779</v>
       </c>
       <c r="D110" s="1"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
-        <v>122</v>
+        <v>12</v>
       </c>
       <c r="B111">
-        <v>-15.446011</v>
+        <v>-15.439249999999999</v>
       </c>
       <c r="C111" s="1">
-        <v>12.029113799999999</v>
+        <v>12.048765</v>
       </c>
       <c r="D111" s="1"/>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
-        <v>61</v>
+        <v>28</v>
       </c>
       <c r="B112">
-        <v>-15.446011</v>
+        <v>-15.435093</v>
       </c>
       <c r="C112" s="1">
-        <v>12.029113799999999</v>
+        <v>12.046393</v>
       </c>
       <c r="D112" s="1"/>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
-        <v>123</v>
+        <v>91</v>
       </c>
       <c r="B113">
-        <v>-15.442837000000001</v>
+        <v>-15.434558000000001</v>
       </c>
       <c r="C113" s="1">
-        <v>12.025421</v>
+        <v>12.046099999999999</v>
       </c>
       <c r="D113" s="1"/>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
-        <v>124</v>
+        <v>61</v>
       </c>
       <c r="B114">
-        <v>-15.442837000000001</v>
+        <v>-15.446011</v>
       </c>
       <c r="C114" s="1">
-        <v>12.025421</v>
+        <v>12.029113799999999</v>
       </c>
       <c r="D114" s="1"/>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
-        <v>62</v>
+        <v>23</v>
       </c>
       <c r="B115">
-        <v>-15.44309</v>
+        <v>-15.435999000000001</v>
       </c>
       <c r="C115" s="1">
-        <v>12.026223</v>
+        <v>12.049841000000001</v>
       </c>
       <c r="D115" s="1"/>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
-        <v>125</v>
+        <v>10</v>
       </c>
       <c r="B116">
-        <v>-15.441784999999999</v>
+        <v>-15.442026</v>
       </c>
       <c r="C116" s="1">
-        <v>12.034478</v>
+        <v>12.048022</v>
       </c>
       <c r="D116" s="1"/>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
-        <v>63</v>
+        <v>110</v>
       </c>
       <c r="B117">
-        <v>-15.441784999999999</v>
+        <v>-15.432672</v>
       </c>
       <c r="C117" s="1">
-        <v>12.034478</v>
+        <v>12.041442</v>
       </c>
       <c r="D117" s="1"/>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
-        <v>64</v>
+        <v>26</v>
       </c>
       <c r="B118">
-        <v>-15.445065</v>
+        <v>-15.440300000000001</v>
       </c>
       <c r="C118" s="1">
-        <v>12.029987999999999</v>
+        <v>12.049073</v>
       </c>
       <c r="D118" s="1"/>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
-        <v>126</v>
+        <v>82</v>
       </c>
       <c r="B119">
-        <v>-15.446236000000001</v>
+        <v>-15.437564999999999</v>
       </c>
       <c r="C119" s="1">
-        <v>12.037397</v>
+        <v>12.047115</v>
       </c>
       <c r="D119" s="1"/>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="B120">
-        <v>-15.447722000000001</v>
+        <v>-15.432672</v>
       </c>
       <c r="C120" s="1">
-        <v>12.028575999999999</v>
+        <v>12.041442</v>
       </c>
       <c r="D120" s="1"/>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
-        <v>128</v>
+        <v>103</v>
       </c>
       <c r="B121">
-        <v>-15.447526</v>
+        <v>-15.437093000000001</v>
       </c>
       <c r="C121" s="1">
-        <v>12.028841999999999</v>
+        <v>12.046369</v>
       </c>
       <c r="D121" s="1"/>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
-        <v>65</v>
+        <v>34</v>
       </c>
       <c r="B122">
-        <v>-15.447526</v>
+        <v>-15.436031</v>
       </c>
       <c r="C122" s="1">
-        <v>12.028841999999999</v>
+        <v>12.046004</v>
       </c>
       <c r="D122" s="1"/>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="B123">
-        <v>-15.447526</v>
+        <v>-15.433439999999999</v>
       </c>
       <c r="C123" s="1">
-        <v>12.028841999999999</v>
+        <v>12.049491</v>
       </c>
       <c r="D123" s="1"/>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
-        <v>129</v>
+        <v>7</v>
       </c>
       <c r="B124">
-        <v>-15.442506</v>
+        <v>-15.437564999999999</v>
       </c>
       <c r="C124" s="1">
-        <v>12.026863000000001</v>
+        <v>12.047115</v>
       </c>
       <c r="D124" s="1"/>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="B125">
-        <v>-15.442506</v>
+        <v>-15.444051999999999</v>
       </c>
       <c r="C125" s="1">
-        <v>12.026863000000001</v>
+        <v>12.036472</v>
       </c>
       <c r="D125" s="1"/>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
-        <v>131</v>
+        <v>57</v>
       </c>
       <c r="B126">
-        <v>-15.44149</v>
+        <v>-15.441229</v>
       </c>
       <c r="C126" s="1">
-        <v>12.025423999999999</v>
+        <v>12.026527</v>
       </c>
       <c r="D126" s="1"/>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
-        <v>67</v>
+        <v>36</v>
       </c>
       <c r="B127">
-        <v>-15.44149</v>
+        <v>-15.436559000000001</v>
       </c>
       <c r="C127" s="1">
-        <v>12.025423999999999</v>
+        <v>12.044413</v>
       </c>
       <c r="D127" s="1"/>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="B128">
-        <v>-15.44149</v>
+        <v>-15.433439999999999</v>
       </c>
       <c r="C128" s="1">
-        <v>12.025423999999999</v>
+        <v>12.049491</v>
       </c>
       <c r="D128" s="1"/>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
-        <v>69</v>
+        <v>87</v>
       </c>
       <c r="B129">
-        <v>-15.44149</v>
+        <v>-15.441048</v>
       </c>
       <c r="C129" s="1">
-        <v>12.025423999999999</v>
+        <v>12.048957</v>
       </c>
       <c r="D129" s="1"/>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="B130">
-        <v>-15.439432</v>
+        <v>-15.437093000000001</v>
       </c>
       <c r="C130" s="1">
-        <v>12.025613</v>
+        <v>12.046369</v>
       </c>
       <c r="D130" s="1"/>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
-        <v>71</v>
+        <v>92</v>
       </c>
       <c r="B131">
-        <v>-15.442218</v>
+        <v>-15.437817000000001</v>
       </c>
       <c r="C131" s="1">
-        <v>12.035133</v>
+        <v>12.045349</v>
       </c>
       <c r="D131" s="1"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:A131" xr:uid="{663AE616-5976-4A00-8446-0A108E968D61}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C131">
+      <sortCondition ref="A1:A131"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>